<commit_message>
Update: finalização da planilha de riscos do projeto
</commit_message>
<xml_diff>
--- a/Planilha e Análise de Riscos.xlsx
+++ b/Planilha e Análise de Riscos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/410ab024c0a0ac41/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Repositório-UMITRIX\UMITRIX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78FBB9C2-4572-4269-AE46-8066E5A7484C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{565A375D-DEB4-4A49-9035-6F66A1C49374}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planiha de riscos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -93,12 +92,96 @@
     <t>Muito Provável 
 (3)</t>
   </si>
+  <si>
+    <t>Planilha de riscos - Umitrix</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Falta de organização e compromisso com o projeto</t>
+  </si>
+  <si>
+    <t>Risco de não entregar todos os requisitos ao fim do projeto</t>
+  </si>
+  <si>
+    <t>Encontrar algum erro no projeto perto da data de entrega</t>
+  </si>
+  <si>
+    <t>Desistência de um membro da equipe</t>
+  </si>
+  <si>
+    <t>Evitar</t>
+  </si>
+  <si>
+    <t>Checagem constante dos requisitos e rotatividade de tarefas, responsábilidades e hierárquias.</t>
+  </si>
+  <si>
+    <t>Manter reuniões diárias constantes (daylis) para envolvimento entre todos os integrantes do projeto. Transparência por parte de todos.</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>Falta de experiência com os recursos e ferramentas utilizadas para execução do projeto</t>
+  </si>
+  <si>
+    <t>Gerir corretamente os requisitos e executa-los dentro dos prazos estabelecidos.</t>
+  </si>
+  <si>
+    <t>Ficarmos desamparados caso algum membro não compareça na apresentação do projeto por motivos pessoais/saúde</t>
+  </si>
+  <si>
+    <t>Todos intregantes estarem cientes e compreenderem cada etapa e processo do projeto.</t>
+  </si>
+  <si>
+    <t>O responsável de cada requisito verificar periodicamente o andamento do próprio. Independetemente da distribuição desses requisitos.</t>
+  </si>
+  <si>
+    <t>Verificação diária por todos membros na organização da ferramenta de gestão (Trello).</t>
+  </si>
+  <si>
+    <t>Auxílio em tarefas tecnicamente mais complexas  por membros com mais experiência em certa ferramenta ou recurso.</t>
+  </si>
+  <si>
+    <t>Ocorrer empecilhos por conta de mal-funcionamento de aparelhos eletrônicos</t>
+  </si>
+  <si>
+    <t>Erros/bugs nas sintaxes dos códigos</t>
+  </si>
+  <si>
+    <t>Fazer revisões nos códigos e correção de possíveis falhas e manter as sintaxes legíveis e limpas. Compreensão de cada bloco de código entre os envolvidos.</t>
+  </si>
+  <si>
+    <t>Entregar algum requisito incondizente com o esperado</t>
+  </si>
+  <si>
+    <t>Alinhamento nas sprint's com o cliente e com o gestor de projetos.</t>
+  </si>
+  <si>
+    <t>Check-up's e testes contínuos dos dispositivos nos treinamentos da apresentação e Backup de todos os requisitos do projeto em outro aparelho.</t>
+  </si>
+  <si>
+    <t>Contato frequente para evitar que haja informações desconexas entre os membros, evitando assim maiores barreiras de comunicação.</t>
+  </si>
+  <si>
+    <t>Má apresentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treinos constantes e feedbacks do grupo. Em questões individuais, gravações própias para conseguir ficar menos ansioso e melhor preparação </t>
+  </si>
+  <si>
+    <t>Deixar a ferramenta de gestão desorganizada (Trello)</t>
+  </si>
+  <si>
+    <t>Dificuldade de comunicação entre a equipe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,15 +190,61 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,8 +269,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -164,37 +305,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,233 +741,436 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1FF0B0-3E60-44FA-8016-C2052E523904}">
-  <dimension ref="A1:N13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="50.77734375" customWidth="1"/>
-    <col min="11" max="14" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="59.83203125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="21.08203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.08203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="106.25" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.6640625" style="1"/>
+    <col min="11" max="14" width="15" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="76.5" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="17.5" customHeight="1" thickBot="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="87.5" customHeight="1" thickBot="1">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6">
+        <f>C4*D4</f>
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="19"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="D5" s="6">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6">
+        <f>C5*D5</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L5" s="16">
         <v>3</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M5" s="17">
         <v>6</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N5" s="17">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="K3" s="4" t="s">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <f>C6*D6</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="7">
-        <v>2</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="L6" s="9">
+        <v>2</v>
+      </c>
+      <c r="M6" s="7">
         <v>4</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N6" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+    <row r="7" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <f>C7*D7</f>
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="M7" s="9">
+        <v>2</v>
+      </c>
+      <c r="N7" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="K4" s="4" t="s">
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A8" s="5">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" ref="E5:E15" si="0">C8*D8</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A9" s="5">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="L4" s="7">
-        <v>1</v>
-      </c>
-      <c r="M4" s="7">
-        <v>2</v>
-      </c>
-      <c r="N4" s="8">
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="L5" s="6" t="s">
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
+      <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="B15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="K4:N4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="936353fbdaa3cfa0ada3a067af0b2a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5658a1d30780e9e89567900e1bf7d795" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -912,24 +1326,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A85FC0E-79F7-49E8-92C5-C8EEEF04D224}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97071F1C-8CB5-4BD1-B0E1-1BFA8268E317}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F454524-A766-4E67-8148-69B670E55CE3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -945,28 +1366,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97071F1C-8CB5-4BD1-B0E1-1BFA8268E317}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A85FC0E-79F7-49E8-92C5-C8EEEF04D224}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>